<commit_message>
Got it to successfully read the scale bar on one test image.
</commit_message>
<xml_diff>
--- a/processed/5pCH4_2247K/kmeans/process_results.xlsx
+++ b/processed/5pCH4_2247K/kmeans/process_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,12 +13,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>fname</t>
   </si>
   <si>
     <t>c3_346a_2247K_4.5atm_0016.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>test_image_1.tif</t>
   </si>
   <si>
     <t>id</t>
@@ -75,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -90,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -99,13 +156,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,85 +180,85 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="true"/>
-    <col min="2" max="2" width="2.90625" customWidth="true"/>
-    <col min="3" max="3" width="6.453125" customWidth="true"/>
-    <col min="4" max="4" width="6.453125" customWidth="true"/>
-    <col min="5" max="5" width="8.453125" customWidth="true"/>
-    <col min="6" max="6" width="8.453125" customWidth="true"/>
-    <col min="7" max="7" width="11.453125" customWidth="true"/>
-    <col min="8" max="8" width="10.453125" customWidth="true"/>
-    <col min="9" max="9" width="11.453125" customWidth="true"/>
-    <col min="10" max="10" width="11.453125" customWidth="true"/>
-    <col min="11" max="11" width="11.453125" customWidth="true"/>
-    <col min="12" max="12" width="11.453125" customWidth="true"/>
-    <col min="13" max="13" width="12.453125" customWidth="true"/>
-    <col min="14" max="14" width="13.453125" customWidth="true"/>
-    <col min="15" max="15" width="13.453125" customWidth="true"/>
-    <col min="16" max="16" width="13.453125" customWidth="true"/>
-    <col min="17" max="17" width="11.453125" customWidth="true"/>
-    <col min="18" max="18" width="11.453125" customWidth="true"/>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="2.85546875" customWidth="true"/>
+    <col min="3" max="3" width="7.140625" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12" customWidth="true"/>
+    <col min="8" max="8" width="11.42578125" customWidth="true"/>
+    <col min="9" max="9" width="11.7109375" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="12" max="12" width="11.7109375" customWidth="true"/>
+    <col min="13" max="13" width="13.7109375" customWidth="true"/>
+    <col min="14" max="14" width="13.7109375" customWidth="true"/>
+    <col min="15" max="15" width="14.28515625" customWidth="true"/>
+    <col min="16" max="16" width="14.28515625" customWidth="true"/>
+    <col min="17" max="17" width="11.7109375" customWidth="true"/>
+    <col min="18" max="18" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -208,54 +267,54 @@
         <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>0.61460000000000004</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E2" s="0">
-        <v>16.594200000000001</v>
+        <v>655.0607287449393</v>
       </c>
       <c r="F2" s="0">
-        <v>13.5212</v>
+        <v>549.79757085020242</v>
       </c>
       <c r="G2" s="0">
-        <v>1.2272727272727273</v>
+        <v>1.1914580265095729</v>
       </c>
       <c r="H2" s="0">
-        <v>468</v>
+        <v>192037</v>
       </c>
       <c r="I2" s="0">
-        <v>15.002738578054823</v>
+        <v>400.38754395112579</v>
       </c>
       <c r="J2" s="0">
-        <v>176.77911888000003</v>
+        <v>125907.32514874852</v>
       </c>
       <c r="K2" s="0">
-        <v>5.4472834345864207</v>
+        <v>214.02914011958359</v>
       </c>
       <c r="L2" s="0">
-        <v>50.604277624898955</v>
+        <v>5261.538461538461</v>
       </c>
       <c r="M2" s="0">
-        <v>0.86749378000655264</v>
+        <v>0.057152517171741753</v>
       </c>
       <c r="N2" s="0">
-        <v>0.14466618873315606</v>
+        <v>0.078196291144331062</v>
       </c>
       <c r="O2" s="0">
-        <v>521.44230769230774</v>
+        <v>334.60599780250681</v>
       </c>
       <c r="P2" s="0">
-        <v>22.963675213675213</v>
+        <v>549.65203059827013</v>
       </c>
       <c r="Q2" s="0">
-        <v>7.2377109635992865</v>
+        <v>25.50559528712196</v>
       </c>
       <c r="R2" s="0">
-        <v>7.2377109635992865</v>
+        <v>25.50559528712196</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -264,54 +323,54 @@
         <v>1</v>
       </c>
       <c r="D3" s="0">
-        <v>0.61460000000000004</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E3" s="0">
-        <v>51.626400000000004</v>
+        <v>295.54655870445345</v>
       </c>
       <c r="F3" s="0">
-        <v>46.709600000000002</v>
+        <v>225.91093117408906</v>
       </c>
       <c r="G3" s="0">
-        <v>1.1052631578947369</v>
+        <v>1.3082437275985663</v>
       </c>
       <c r="H3" s="0">
-        <v>3185</v>
+        <v>49618</v>
       </c>
       <c r="I3" s="0">
-        <v>39.138333860720635</v>
+        <v>203.52029763931074</v>
       </c>
       <c r="J3" s="0">
-        <v>1203.0801146000001</v>
+        <v>32531.593699290264</v>
       </c>
       <c r="K3" s="0">
-        <v>16.729778708853676</v>
+        <v>82.333224198312294</v>
       </c>
       <c r="L3" s="0">
-        <v>154.31268401894513</v>
+        <v>1410.5263157894738</v>
       </c>
       <c r="M3" s="0">
-        <v>0.634893911327848</v>
+        <v>0.20547208005607173</v>
       </c>
       <c r="N3" s="0">
-        <v>0.10257153392329219</v>
+        <v>0.34600305427999284</v>
       </c>
       <c r="O3" s="0">
-        <v>39.680376766091051</v>
+        <v>839.22759885525409</v>
       </c>
       <c r="P3" s="0">
-        <v>71.808163265306121</v>
+        <v>468.38020476439999</v>
       </c>
       <c r="Q3" s="0">
-        <v>15.293940501186157</v>
+        <v>30.221590338439693</v>
       </c>
       <c r="R3" s="0">
-        <v>15.293940501186157</v>
+        <v>30.221590338439693</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -320,54 +379,54 @@
         <v>1</v>
       </c>
       <c r="D4" s="0">
-        <v>0.61460000000000004</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E4" s="0">
-        <v>6.7606000000000002</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F4" s="0">
-        <v>6.7606000000000002</v>
+        <v>6.4777327935222671</v>
       </c>
       <c r="G4" s="0">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="0">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I4" s="0">
-        <v>7.5333582157649577</v>
+        <v>9.5826239234059862</v>
       </c>
       <c r="J4" s="0">
-        <v>44.572512880000005</v>
+        <v>72.120506810470573</v>
       </c>
       <c r="K4" s="0">
-        <v>2.66608784423439</v>
+        <v>3.5330940923602463</v>
       </c>
       <c r="L4" s="0">
-        <v>24.81516963107827</v>
+        <v>31.247639500791408</v>
       </c>
       <c r="M4" s="0">
-        <v>0.90958331783489166</v>
+        <v>0.92818426720588398</v>
       </c>
       <c r="N4" s="0">
-        <v>0.35415353647562148</v>
+        <v>0.18568268190298765</v>
       </c>
       <c r="O4" s="0">
-        <v>884.23728813559319</v>
+        <v>317.92727272727274</v>
       </c>
       <c r="P4" s="0">
-        <v>46.203389830508478</v>
+        <v>616.25454545454545</v>
       </c>
       <c r="Q4" s="0">
-        <v>2.3919666269368296</v>
+        <v>6.851449106449107</v>
       </c>
       <c r="R4" s="0">
-        <v>2.3919666269368296</v>
+        <v>6.851449106449107</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0">
         <v>4</v>
@@ -376,49 +435,49 @@
         <v>1</v>
       </c>
       <c r="D5" s="0">
-        <v>0.61460000000000004</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E5" s="0">
-        <v>324.50880000000001</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="F5" s="0">
-        <v>285.17439999999999</v>
+        <v>8.9068825910931171</v>
       </c>
       <c r="G5" s="0">
-        <v>1.1379310344827587</v>
+        <v>1.1818181818181817</v>
       </c>
       <c r="H5" s="0">
-        <v>81613</v>
+        <v>107</v>
       </c>
       <c r="I5" s="0">
-        <v>198.11952879665927</v>
+        <v>9.4510484721611245</v>
       </c>
       <c r="J5" s="0">
-        <v>30827.936387080004</v>
+        <v>70.15358389745775</v>
       </c>
       <c r="K5" s="0">
-        <v>110.70975222919606</v>
+        <v>3.7963541089374435</v>
       </c>
       <c r="L5" s="0">
-        <v>1635.1300655277334</v>
+        <v>34.355278485492676</v>
       </c>
       <c r="M5" s="0">
-        <v>0.14489376916506391</v>
+        <v>0.74691774936711841</v>
       </c>
       <c r="N5" s="0">
-        <v>0.19412657574283426</v>
+        <v>0.20968532818614247</v>
       </c>
       <c r="O5" s="0">
-        <v>543.52446301447071</v>
+        <v>550.8878504672897</v>
       </c>
       <c r="P5" s="0">
-        <v>520.44502714028397</v>
+        <v>629.12149532710282</v>
       </c>
       <c r="Q5" s="0">
-        <v>28.420331970466144</v>
+        <v>3.3691803278688521</v>
       </c>
       <c r="R5" s="0">
-        <v>28.420331970466144</v>
+        <v>3.3691803278688521</v>
       </c>
     </row>
     <row r="6">

</xml_diff>